<commit_message>
EnterpriseAcctSetup_IP code added, BVT5 fine tuning
</commit_message>
<xml_diff>
--- a/LyndaTestAutomationFramework/LyndaTestAutomationFramework/Tests/Public_AcctAccessData.xlsx
+++ b/LyndaTestAutomationFramework/LyndaTestAutomationFramework/Tests/Public_AcctAccessData.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -48,7 +48,7 @@
     <t>4-12-2012-37321</t>
   </si>
   <si>
-    <t>5-11-2012-52547</t>
+    <t>5-30-2012-35529</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="B1:AO5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>